<commit_message>
Creación de Dao y DaoImpl
Se actualiza modelo E-R. Se crean las clases e implementan interfaces
de DAOs.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/bd/inserts.xlsx
+++ b/src/main/webapp/WEB-INF/bd/inserts.xlsx
@@ -19,7 +19,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="201">
+  <si>
+    <t>'ROLE_ROOT'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>acompaniante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_acompaniante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'root'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'ROLE_ADMIN'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'admin'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>'2016-01-03'</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -45,11 +69,167 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>empresa_tarjeta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_empresa_tarjeta</t>
+    <t>costo_congresista</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_costo_congresista</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-01-01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-02-29'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-03-01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-04-30'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-05-01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-06-30'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_mesa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num_personas_habitacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por día. Incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por 2 días. Incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por 3 días. Incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por día. Incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por 2 días. Incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación sencilla por día. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación sencilla por 2 días. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación sencilla por 3 días. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por día. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por 2 días. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Habitación doble por 3 días. NO incluye desayuno'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Doble 1 día'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Masonería en Constituciones'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Derechos Humanos'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Masonería y Educación'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Globalización Económica y Soberanía'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Libertad de Creencias y Estado Laíco'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'14º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'4º - 13º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'15º - 18º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'19º - 30º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>costo_acompaniante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_costo_acompaniante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_parametro_configuracion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valor_int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -57,19 +237,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>'VISA'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Master Card'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_tarjeta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_tarjeta</t>
+    <t>id_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'31º- 32º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º S.·. N.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º M.·. A.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º M.·. Past-A.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grado_pretende</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado_pretende</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -77,31 +273,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>precio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>activo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>'Crédito'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Débito'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>costo_congresista</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_costo_congresista</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_fin</t>
+    <t>'14º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'15º - 18º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'19º - 30º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'31º - 32º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>' '</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paquete_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_paquete_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -109,43 +325,294 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>'2016-01-01'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-02-29'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-03-01'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-04-30'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-05-01'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-06-30'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>costo_acompañante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_costo_acompañante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_fin</t>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Lalo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Mario'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Oaxaca'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Puebla'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Querétaro'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>' '</t>
+  </si>
+  <si>
+    <t>' '</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Quintana Roo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'San Luis Potosí'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Sinaloa'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Sonora'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tabasco'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tamaulipas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tlaxcala'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Veracruz de Ignacio de la Llave'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Yucatán'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Zacatecas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Chiapas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Chihuahua'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ciudad de México'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_ponencia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_ponencia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Durango'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Guanajuato'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Guerrero'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Hidalgo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Jalisco'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'México'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Michoacán de Ocampo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Morelos'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Nayarit'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Nuevo León'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contrasenia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_entrada</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'gmho'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Holiday Inn Plaza Universidad (Sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Gerardo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ninguna en particular'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Aguascalientes'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Baja California Sur'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Baja California'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Campeche'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Coahuila de Zaragoza'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Colima'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ap_paterno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ap_materno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Gerardo Martín'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Hernández'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Oliva'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_mesa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -153,115 +620,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>num_personas_habitacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por día. Incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por 2 días. Incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por 3 días. Incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por día. Incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por 2 días. Incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación sencilla por día. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación sencilla por 2 días. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación sencilla por 3 días. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por día. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por 2 días. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Habitación doble por 3 días. NO incluye desayuno'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Doble 1 día'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ninguna en especial'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Masonería en Constituciones'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Derechos Humanos'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Masonería y Educación'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Globalización Económica y Soberanía'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Libertad de Creencias y Estado Laíco'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'14º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'4º - 13º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'15º - 18º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'19º - 30º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'31º- 32º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º S.·. N.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º M.·. A.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º M.·. Past-A.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grado_pretende</t>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'contador_visitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perfil_x_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil_x_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ramada Inn Vía Venetto (Sub-sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'City Express Patio Universiad (Sub-sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>registro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_registro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre_cuerpo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delegacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hospedaje</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_hospedaje</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_salida</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-01-02'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colacion_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_colacion_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cuerpo_pretende</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -269,11 +736,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>'Cocodrilitos'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Abejitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Plantitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importe_pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nombre</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>precio</t>
+    <t>descripcion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -281,509 +780,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>'14º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'15º - 18º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'19º - 30º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'31º - 32º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>' '</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>paquete_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_paquete_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>precio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Lalo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Mario'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Oaxaca'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Puebla'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Querétaro'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>' '</t>
-  </si>
-  <si>
-    <t>' '</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Quintana Roo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'San Luis Potosí'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Sinaloa'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Sonora'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tabasco'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tamaulipas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tlaxcala'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Veracruz de Ignacio de la Llave'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Yucatán'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Zacatecas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Chiapas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Chihuahua'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ciudad de México'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_ponencia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_ponencia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Durango'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Guanajuato'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Guerrero'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Hidalgo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Jalisco'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'México'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Michoacán de Ocampo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Morelos'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Nayarit'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Nuevo León'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>contrasenia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_entrada</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'gmho'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'ROLE_ROOT'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>acompaniante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_acompaniante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'root'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'ROLE_ADMIN'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'admin'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Aguascalientes'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Baja California Sur'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Baja California'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Campeche'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Coahuila de Zaragoza'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Colima'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ap_paterno</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ap_materno</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Gerardo Martín'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Hernández'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Oliva'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_mesa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_mesa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'contador_visitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>perfil_x_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil_x_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ramada Inn Vía Venetto (Sub-sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'City Express Patio Universiad (Sub-sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>registro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_registro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre_cuerpo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delegacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hospedaje</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hospedaje</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_salida</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-01-02'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>colacion_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_colacion_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cuerpo_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Cocodrilitos'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Abejitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Plantitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>importe_pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>'Congresista'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -825,50 +821,6 @@
   </si>
   <si>
     <t>parametro_configuracion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_parametro_configuracion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>valor_int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Holiday Inn Plaza Universidad (Sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Gerardo'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1240,10 +1192,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A3:J183"/>
+  <dimension ref="A3:J171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1334,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1352,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1377,13 +1329,13 @@
         <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>210</v>
+        <v>133</v>
       </c>
       <c r="D14" t="s">
-        <v>211</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>209</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1928,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D56" t="s">
         <v>84</v>
@@ -1946,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D57" t="s">
         <v>84</v>
@@ -1964,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D58" t="s">
         <v>84</v>
@@ -1982,7 +1934,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D59" t="s">
         <v>84</v>
@@ -2069,21 +2021,21 @@
     </row>
     <row r="66" spans="1:5">
       <c r="B66" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="B67" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" t="s">
         <v>187</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>188</v>
       </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>189</v>
-      </c>
-      <c r="E67" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2095,7 +2047,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D68" t="s">
         <v>84</v>
@@ -2113,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D69" t="s">
         <v>84</v>
@@ -2131,7 +2083,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D70" t="s">
         <v>84</v>
@@ -2149,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D71" t="s">
         <v>84</v>
@@ -2167,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D72" t="s">
         <v>84</v>
@@ -2185,7 +2137,7 @@
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D73" t="s">
         <v>84</v>
@@ -2204,13 +2156,13 @@
         <v>100</v>
       </c>
       <c r="C77" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" t="s">
         <v>188</v>
       </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>189</v>
-      </c>
-      <c r="E77" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2222,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>85</v>
@@ -2240,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>85</v>
@@ -2258,7 +2210,7 @@
         <v>3</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>85</v>
@@ -2299,13 +2251,13 @@
     <row r="85" spans="1:6">
       <c r="A85" t="str">
         <f>CONCATENATE("INSERT INTO ",B$83," (",B$84,", ",C$84,", ",D$84,", ",E$84,") VALUES (",B85,",",C85,",",D85,",",E85,");" )</f>
-        <v>INSERT INTO tipo_mesa (id_tipo_mesa, nombre, descripcion, activo) VALUES (1,'Ninguna en especial',' ',1);</v>
+        <v>INSERT INTO tipo_mesa (id_tipo_mesa, nombre, descripcion, activo) VALUES (1,'Ninguna en particular',' ',1);</v>
       </c>
       <c r="B85">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>85</v>
@@ -2323,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>85</v>
@@ -2341,7 +2293,7 @@
         <v>3</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>85</v>
@@ -2359,7 +2311,7 @@
         <v>4</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>85</v>
@@ -2377,7 +2329,7 @@
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>85</v>
@@ -2395,7 +2347,7 @@
         <v>6</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>85</v>
@@ -2530,18 +2482,18 @@
     </row>
     <row r="101" spans="1:7">
       <c r="B101" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="B102" t="s">
-        <v>206</v>
+        <v>54</v>
       </c>
       <c r="C102" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D102" t="s">
-        <v>207</v>
+        <v>55</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2553,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>208</v>
+        <v>131</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -2633,10 +2585,10 @@
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F110">
         <v>3520</v>
@@ -2657,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F111">
         <v>7040</v>
@@ -2681,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F112">
         <v>10560</v>
@@ -2705,10 +2657,10 @@
         <v>2</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F113">
         <v>1561</v>
@@ -2729,10 +2681,10 @@
         <v>2</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F114">
         <v>3122</v>
@@ -2753,10 +2705,10 @@
         <v>2</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F115">
         <v>4683</v>
@@ -2777,10 +2729,10 @@
         <v>3</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F116">
         <v>895</v>
@@ -2801,10 +2753,10 @@
         <v>3</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F117">
         <v>1790</v>
@@ -2825,10 +2777,10 @@
         <v>3</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F118">
         <v>2685</v>
@@ -2849,10 +2801,10 @@
         <v>3</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F119">
         <v>1265</v>
@@ -2873,10 +2825,10 @@
         <v>3</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F120">
         <v>2530</v>
@@ -2897,10 +2849,10 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F121">
         <v>3795</v>
@@ -2921,7 +2873,7 @@
     </row>
     <row r="124" spans="1:7">
       <c r="B124" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2929,58 +2881,83 @@
     </row>
     <row r="125" spans="1:7">
       <c r="B125" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="D125" t="s">
-        <v>151</v>
+        <v>15</v>
       </c>
       <c r="E125" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="F125" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$124," (",B$125,", ",C$125,", ",D$125,", ",E$125,") VALUES (",B126,",",C126,",",D126,",",E126,");" )</f>
-        <v>INSERT INTO empresa_tarjeta (id_empresa_tarjeta, nombre, descripcion, activo) VALUES (1,'VISA',' ',1);</v>
+        <f>CONCATENATE("INSERT INTO ",B$124," (",B$125,", ",C$125,", ",D$125,", ",E$125,", ",F$125,") VALUES (",B126,",",C126,",",D126,",",E126,",",F126,");" )</f>
+        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (1,'2016-01-01','2016-02-29',1800,1);</v>
       </c>
       <c r="B126">
         <v>1</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="E126" s="1">
+        <v>1800</v>
+      </c>
+      <c r="F126">
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:7">
       <c r="A127" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$124," (",B$125,", ",C$125,", ",D$125,", ",E$125,") VALUES (",B127,",",C127,",",D127,",",E127,");" )</f>
-        <v>INSERT INTO empresa_tarjeta (id_empresa_tarjeta, nombre, descripcion, activo) VALUES (2,'Master Card',' ',1);</v>
+        <f t="shared" ref="A127:A128" si="8">CONCATENATE("INSERT INTO ",B$124," (",B$125,", ",C$125,", ",D$125,", ",E$125,", ",F$125,") VALUES (",B127,",",C127,",",D127,",",E127,",",F127,");" )</f>
+        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (2,'2016-03-01','2016-04-30',2300,1);</v>
       </c>
       <c r="B127">
         <v>2</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="E127" s="1">
+        <v>2300</v>
+      </c>
+      <c r="F127">
         <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:7">
-      <c r="C128" s="1"/>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
+      <c r="A128" t="str">
+        <f t="shared" si="8"/>
+        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (3,'2016-05-01','2016-06-30',2800,1);</v>
+      </c>
+      <c r="B128">
+        <v>3</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E128" s="1">
+        <v>2800</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
     </row>
     <row r="129" spans="1:6">
       <c r="C129" s="1"/>
@@ -2988,601 +2965,432 @@
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:6">
-      <c r="B130" t="s">
-        <v>11</v>
-      </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
     </row>
     <row r="131" spans="1:6">
       <c r="B131" t="s">
-        <v>12</v>
-      </c>
-      <c r="C131" t="s">
-        <v>13</v>
-      </c>
-      <c r="D131" t="s">
-        <v>151</v>
-      </c>
-      <c r="E131" t="s">
-        <v>14</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$130," (",B$131,", ",C$131,", ",D$131,", ",E$131,") VALUES (",B132,",",C132,",",D132,",",E132,");" )</f>
-        <v>INSERT INTO tipo_tarjeta (id_tipo_tarjeta, nombre, descripcion, activo) VALUES (1,'Crédito',' ',1);</v>
-      </c>
-      <c r="B132">
-        <v>1</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E132" s="1">
-        <v>1</v>
+      <c r="B132" t="s">
+        <v>49</v>
+      </c>
+      <c r="C132" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" t="s">
+        <v>24</v>
+      </c>
+      <c r="E132" t="s">
+        <v>63</v>
+      </c>
+      <c r="F132" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$130," (",B$131,", ",C$131,", ",D$131,", ",E$131,") VALUES (",B133,",",C133,",",D133,",",E133,");" )</f>
-        <v>INSERT INTO tipo_tarjeta (id_tipo_tarjeta, nombre, descripcion, activo) VALUES (2,'Débito',' ',1);</v>
+        <f>CONCATENATE("INSERT INTO ",B$131," (",B$132,", ",C$132,", ",D$132,", ",E$132,", ",F$132,") VALUES (",B133,",",C133,",",D133,",",E133,",",F133,");" )</f>
+        <v>INSERT INTO costo_acompaniante (id_costo_acompaniante, fecha_inicio, fecha_fin, precio, activo) VALUES (1,'2016-01-01','2016-02-29',1500,1);</v>
       </c>
       <c r="B133">
+        <v>1</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E133" s="1">
+        <v>1500</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" t="str">
+        <f t="shared" ref="A134:A135" si="9">CONCATENATE("INSERT INTO ",B$131," (",B$132,", ",C$132,", ",D$132,", ",E$132,", ",F$132,") VALUES (",B134,",",C134,",",D134,",",E134,",",F134,");" )</f>
+        <v>INSERT INTO costo_acompaniante (id_costo_acompaniante, fecha_inicio, fecha_fin, precio, activo) VALUES (2,'2016-03-01','2016-04-30',2000,1);</v>
+      </c>
+      <c r="B134">
         <v>2</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E133" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
+      <c r="C134" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E134" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" spans="1:6">
-      <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="B136" t="s">
-        <v>17</v>
-      </c>
-      <c r="C136" s="1"/>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="B137" t="s">
-        <v>18</v>
-      </c>
-      <c r="C137" t="s">
-        <v>19</v>
-      </c>
-      <c r="D137" t="s">
-        <v>20</v>
-      </c>
-      <c r="E137" t="s">
+      <c r="A135" t="str">
+        <f t="shared" si="9"/>
+        <v>INSERT INTO costo_acompaniante (id_costo_acompaniante, fecha_inicio, fecha_fin, precio, activo) VALUES (3,'2016-05-01','2016-06-30',2500,1);</v>
+      </c>
+      <c r="B135">
+        <v>3</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F137" t="s">
-        <v>152</v>
+      <c r="D135" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E135" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$136," (",B$137,", ",C$137,", ",D$137,", ",E$137,", ",F$137,") VALUES (",B138,",",C138,",",D138,",",E138,",",F138,");" )</f>
-        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (1,'2016-01-01','2016-02-29',1800,1);</v>
-      </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E138" s="1">
-        <v>1800</v>
-      </c>
-      <c r="F138">
-        <v>1</v>
+      <c r="B138" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" t="str">
-        <f t="shared" ref="A139:A140" si="8">CONCATENATE("INSERT INTO ",B$136," (",B$137,", ",C$137,", ",D$137,", ",E$137,", ",F$137,") VALUES (",B139,",",C139,",",D139,",",E139,",",F139,");" )</f>
-        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (2,'2016-03-01','2016-04-30',2300,1);</v>
-      </c>
-      <c r="B139">
-        <v>2</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E139" s="1">
-        <v>2300</v>
-      </c>
-      <c r="F139">
-        <v>1</v>
+      <c r="B139" t="s">
+        <v>155</v>
+      </c>
+      <c r="C139" t="s">
+        <v>156</v>
+      </c>
+      <c r="D139" t="s">
+        <v>157</v>
+      </c>
+      <c r="E139" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="str">
-        <f t="shared" si="8"/>
-        <v>INSERT INTO costo_congresista (id_costo_congresista, fecha_inicio, fecha_fin, precio, activo) VALUES (3,'2016-05-01','2016-06-30',2800,1);</v>
+        <f>CONCATENATE("INSERT INTO ",B$138," (",B$139,", ",C$139,", ",D$139,", ",E$139,") VALUES (",B140,",",C140,",",D140,",",E140,");" )</f>
+        <v>INSERT INTO participante (id_participante, nombre, id_estado, activo) VALUES (1,'Gerardo',1,1);</v>
       </c>
       <c r="B140">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E140" s="1">
-        <v>2800</v>
-      </c>
-      <c r="F140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:6">
       <c r="B143" t="s">
-        <v>28</v>
-      </c>
-      <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="144" spans="1:6">
       <c r="B144" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D144" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E144" t="s">
-        <v>63</v>
-      </c>
-      <c r="F144" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$143," (",B$144,", ",C$144,", ",D$144,", ",E$144,", ",F$144,") VALUES (",B145,",",C145,",",D145,",",E145,",",F145,");" )</f>
-        <v>INSERT INTO costo_acompañante (id_costo_acompañante, fecha_inicio, fecha_fin, precio, activo) VALUES (1,'2016-01-01','2016-02-29',1500,1);</v>
+        <f>CONCATENATE("INSERT INTO ",B$143," (",B$144,", ",C$144,", ",D$144,", ",E$144,") VALUES (",B145,",",C145,",",D145,",",E145,");" )</f>
+        <v>INSERT INTO acompaniante (id_acompaniante, id_participante, nombre, activo) VALUES (1,1,'Lalo',1);</v>
       </c>
       <c r="B145">
         <v>1</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>22</v>
+      <c r="C145">
+        <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E145" s="1">
-        <v>1500</v>
-      </c>
-      <c r="F145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+        <v>79</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146" t="str">
-        <f t="shared" ref="A146:A147" si="9">CONCATENATE("INSERT INTO ",B$143," (",B$144,", ",C$144,", ",D$144,", ",E$144,", ",F$144,") VALUES (",B146,",",C146,",",D146,",",E146,",",F146,");" )</f>
-        <v>INSERT INTO costo_acompañante (id_costo_acompañante, fecha_inicio, fecha_fin, precio, activo) VALUES (2,'2016-03-01','2016-04-30',2000,1);</v>
+        <f>CONCATENATE("INSERT INTO ",B$143," (",B$144,", ",C$144,", ",D$144,", ",E$144,") VALUES (",B146,",",C146,",",D146,",",E146,");" )</f>
+        <v>INSERT INTO acompaniante (id_acompaniante, id_participante, nombre, activo) VALUES (2,1,'Mario',1);</v>
       </c>
       <c r="B146">
         <v>2</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>24</v>
+      <c r="C146">
+        <v>1</v>
       </c>
       <c r="D146" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
+      <c r="B149" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="B150" t="s">
+        <v>163</v>
+      </c>
+      <c r="C150" t="s">
+        <v>164</v>
+      </c>
+      <c r="D150" t="s">
+        <v>165</v>
+      </c>
+      <c r="E150" t="s">
+        <v>166</v>
+      </c>
+      <c r="F150" t="s">
+        <v>167</v>
+      </c>
+      <c r="G150" t="s">
+        <v>168</v>
+      </c>
+      <c r="H150" t="s">
+        <v>100</v>
+      </c>
+      <c r="I150" t="s">
         <v>25</v>
       </c>
-      <c r="E146" s="1">
+      <c r="J150" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="A151" t="str">
+        <f>CONCATENATE("INSERT INTO ",B$149," (",B$150,", ",C$150,", ",D$150,", ",E$150,", ",F$150,", ",G$150,", ",H$150,", ",I$150,", ",J$150,") VALUES (",B151,",",C151,",",D151,",",E151,",",F151,",",G151,",",H151,",",I151,",",J151,");" )</f>
+        <v>INSERT INTO registro (id_registro, id_participante, id_grado, nombre_cuerpo, delegacion, id_tipo_participacion, id_tipo_ponencia, id_tipo_mesa, activo) VALUES (1,1,1,'Abejitas','Plantitas',1,3,1,1);</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F151" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+      <c r="I151">
+        <v>1</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
+      <c r="B154" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
+      <c r="B155" t="s">
+        <v>170</v>
+      </c>
+      <c r="C155" t="s">
+        <v>171</v>
+      </c>
+      <c r="D155" t="s">
+        <v>71</v>
+      </c>
+      <c r="E155" t="s">
+        <v>115</v>
+      </c>
+      <c r="F155" t="s">
+        <v>172</v>
+      </c>
+      <c r="G155" t="s">
+        <v>26</v>
+      </c>
+      <c r="H155" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" t="str">
+        <f>CONCATENATE("INSERT INTO ",B$154," (",B$155,", ",C$155,", ",D$155,", ",E$155,", ",F$155,", ",G$155,", ",H$155,") VALUES (",B156,",",C156,",",D156,",",E156,",",F156,",",G156,",",H156,");" )</f>
+        <v>INSERT INTO hospedaje (id_hospedaje, id_participante, id_paquete_hotel, fecha_entrada, fecha_salida, num_personas_habitacion, activo) VALUES (1,1,1,'2016-01-02','2016-01-03',1,1);</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F156" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
+      <c r="B159" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
+      <c r="B160" t="s">
+        <v>175</v>
+      </c>
+      <c r="C160" t="s">
+        <v>176</v>
+      </c>
+      <c r="D160" t="s">
+        <v>178</v>
+      </c>
+      <c r="E160" t="s">
+        <v>177</v>
+      </c>
+      <c r="F160" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" t="str">
+        <f>CONCATENATE("INSERT INTO ",B$159," (",B$160,", ",C$160,", ",D$160,", ",E$160,", ",F$160,") VALUES (",B161,",",C161,",",D161,",",E161,",",F161,");" )</f>
+        <v>INSERT INTO colacion_grado (id_colacion_grado, id_participante, id_grado_pretende, cuerpo_pretende, activo) VALUES (1,1,2,'Cocodrilitos',1);</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="D161" s="1">
+        <v>2</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="B164" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="B165" t="s">
+        <v>183</v>
+      </c>
+      <c r="C165" t="s">
+        <v>176</v>
+      </c>
+      <c r="D165" t="s">
+        <v>184</v>
+      </c>
+      <c r="E165" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" t="str">
+        <f>CONCATENATE("INSERT INTO ",B$164," (",B$165,", ",C$165,", ",D$165,", ",E$165,") VALUES (",B166,",",C166,",",D166,",",E166,");" )</f>
+        <v>INSERT INTO pago (id_pago, id_participante, importe_pago, activo) VALUES (1,1,2000,1);</v>
+      </c>
+      <c r="B166">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="D166">
         <v>2000</v>
       </c>
-      <c r="F146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" t="str">
-        <f t="shared" si="9"/>
-        <v>INSERT INTO costo_acompañante (id_costo_acompañante, fecha_inicio, fecha_fin, precio, activo) VALUES (3,'2016-05-01','2016-06-30',2500,1);</v>
-      </c>
-      <c r="B147">
-        <v>3</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E147" s="1">
-        <v>2500</v>
-      </c>
-      <c r="F147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="B150" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="B151" t="s">
-        <v>155</v>
-      </c>
-      <c r="C151" t="s">
-        <v>156</v>
-      </c>
-      <c r="D151" t="s">
-        <v>157</v>
-      </c>
-      <c r="E151" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$150," (",B$151,", ",C$151,", ",D$151,", ",E$151,") VALUES (",B152,",",C152,",",D152,",",E152,");" )</f>
-        <v>INSERT INTO participante (id_participante, nombre, id_estado, activo) VALUES (1,'Gerardo',1,1);</v>
-      </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D152">
-        <v>1</v>
-      </c>
-      <c r="E152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="B155" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="B156" t="s">
-        <v>133</v>
-      </c>
-      <c r="C156" t="s">
-        <v>77</v>
-      </c>
-      <c r="D156" t="s">
-        <v>78</v>
-      </c>
-      <c r="E156" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$155," (",B$156,", ",C$156,", ",D$156,", ",E$156,") VALUES (",B157,",",C157,",",D157,",",E157,");" )</f>
-        <v>INSERT INTO acompaniante (id_acompaniante, id_participante, nombre, activo) VALUES (1,1,'Lalo',1);</v>
-      </c>
-      <c r="B157">
-        <v>1</v>
-      </c>
-      <c r="C157">
-        <v>1</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="A158" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$155," (",B$156,", ",C$156,", ",D$156,", ",E$156,") VALUES (",B158,",",C158,",",D158,",",E158,");" )</f>
-        <v>INSERT INTO acompaniante (id_acompaniante, id_participante, nombre, activo) VALUES (2,1,'Mario',1);</v>
-      </c>
-      <c r="B158">
-        <v>2</v>
-      </c>
-      <c r="C158">
-        <v>1</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:10">
-      <c r="B161" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10">
-      <c r="B162" t="s">
-        <v>163</v>
-      </c>
-      <c r="C162" t="s">
-        <v>164</v>
-      </c>
-      <c r="D162" t="s">
-        <v>165</v>
-      </c>
-      <c r="E162" t="s">
-        <v>166</v>
-      </c>
-      <c r="F162" t="s">
-        <v>167</v>
-      </c>
-      <c r="G162" t="s">
-        <v>168</v>
-      </c>
-      <c r="H162" t="s">
-        <v>100</v>
-      </c>
-      <c r="I162" t="s">
-        <v>32</v>
-      </c>
-      <c r="J162" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="163" spans="1:10">
-      <c r="A163" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$161," (",B$162,", ",C$162,", ",D$162,", ",E$162,", ",F$162,", ",G$162,", ",H$162,", ",I$162,", ",J$162,") VALUES (",B163,",",C163,",",D163,",",E163,",",F163,",",G163,",",H163,",",I163,",",J163,");" )</f>
-        <v>INSERT INTO registro (id_registro, id_participante, id_grado, nombre_cuerpo, delegacion, id_tipo_participacion, id_tipo_ponencia, id_tipo_mesa, activo) VALUES (1,1,1,'Abejitas','Plantitas',1,3,1,1);</v>
-      </c>
-      <c r="B163">
-        <v>1</v>
-      </c>
-      <c r="C163">
-        <v>1</v>
-      </c>
-      <c r="D163">
-        <v>1</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G163">
-        <v>1</v>
-      </c>
-      <c r="H163">
-        <v>3</v>
-      </c>
-      <c r="I163">
-        <v>1</v>
-      </c>
-      <c r="J163">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10">
-      <c r="B166" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10">
-      <c r="B167" t="s">
-        <v>170</v>
-      </c>
-      <c r="C167" t="s">
-        <v>171</v>
-      </c>
-      <c r="D167" t="s">
-        <v>172</v>
-      </c>
-      <c r="E167" t="s">
-        <v>71</v>
-      </c>
-      <c r="F167" t="s">
-        <v>115</v>
-      </c>
-      <c r="G167" t="s">
-        <v>173</v>
-      </c>
-      <c r="H167" t="s">
-        <v>33</v>
-      </c>
-      <c r="I167" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
-      <c r="A168" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$166," (",B$167,", ",C$167,", ",D$167,", ",E$167,", ",F$167,", ",G$167,", ",H$167,", ",I$167,") VALUES (",B168,",",C168,",",D168,",",E168,",",F168,",",G168,",",H168,",",I168,");" )</f>
-        <v>INSERT INTO hospedaje (id_hospedaje, id_participante, id_hotel, id_paquete_hotel, fecha_entrada, fecha_salida, num_personas_habitacion, activo) VALUES (1,1,1,1,'2016-01-02','2016-01-03',1,1);</v>
-      </c>
-      <c r="B168">
-        <v>1</v>
-      </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-      <c r="D168">
-        <v>1</v>
-      </c>
-      <c r="E168">
-        <v>1</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G168" s="2" t="s">
+      <c r="E166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="B169" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="B170" t="s">
+        <v>50</v>
+      </c>
+      <c r="C170" t="s">
+        <v>51</v>
+      </c>
+      <c r="D170" t="s">
+        <v>52</v>
+      </c>
+      <c r="E170" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" t="str">
+        <f>CONCATENATE("INSERT INTO ",B$169," (",B$170,", ",C$170,", ",D$170,", ",E$170,") VALUES (",B171,",",C171,",",D171,",",E171,");" )</f>
+        <v>INSERT INTO parametro_configuracion (id_parametro_configuracion, nombre, valor_int, activo) VALUES (1,'contador_visitas',0,1);</v>
+      </c>
+      <c r="B171">
+        <v>1</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D171">
         <v>0</v>
       </c>
-      <c r="H168">
-        <v>1</v>
-      </c>
-      <c r="I168">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10">
-      <c r="B171" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10">
-      <c r="B172" t="s">
-        <v>176</v>
-      </c>
-      <c r="C172" t="s">
-        <v>177</v>
-      </c>
-      <c r="D172" t="s">
-        <v>179</v>
-      </c>
-      <c r="E172" t="s">
-        <v>178</v>
-      </c>
-      <c r="F172" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="173" spans="1:10">
-      <c r="A173" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$171," (",B$172,", ",C$172,", ",D$172,", ",E$172,", ",F$172,") VALUES (",B173,",",C173,",",D173,",",E173,",",F173,");" )</f>
-        <v>INSERT INTO colacion_grado (id_colacion_grado, id_participante, id_grado_pretende, cuerpo_pretende, activo) VALUES (1,1,2,'Cocodrilitos',1);</v>
-      </c>
-      <c r="B173">
-        <v>1</v>
-      </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-      <c r="D173" s="1">
-        <v>2</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F173">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="1:10">
-      <c r="B176" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
-      <c r="B177" t="s">
-        <v>184</v>
-      </c>
-      <c r="C177" t="s">
-        <v>177</v>
-      </c>
-      <c r="D177" t="s">
-        <v>185</v>
-      </c>
-      <c r="E177" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5">
-      <c r="A178" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$176," (",B$177,", ",C$177,", ",D$177,", ",E$177,") VALUES (",B178,",",C178,",",D178,",",E178,");" )</f>
-        <v>INSERT INTO pago (id_pago, id_participante, importe_pago, activo) VALUES (1,1,2000,1);</v>
-      </c>
-      <c r="B178">
-        <v>1</v>
-      </c>
-      <c r="C178">
-        <v>1</v>
-      </c>
-      <c r="D178">
-        <v>2000</v>
-      </c>
-      <c r="E178">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5">
-      <c r="B181" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5">
-      <c r="B182" t="s">
-        <v>202</v>
-      </c>
-      <c r="C182" t="s">
-        <v>203</v>
-      </c>
-      <c r="D182" t="s">
-        <v>204</v>
-      </c>
-      <c r="E182" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5">
-      <c r="A183" t="str">
-        <f>CONCATENATE("INSERT INTO ",B$181," (",B$182,", ",C$182,", ",D$182,", ",E$182,") VALUES (",B183,",",C183,",",D183,",",E183,");" )</f>
-        <v>INSERT INTO parametro_configuracion (id_parametro_configuracion, nombre, valor_int, activo) VALUES (1,'contador_visitas',0,1);</v>
-      </c>
-      <c r="B183">
-        <v>1</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D183">
-        <v>0</v>
-      </c>
-      <c r="E183">
+      <c r="E171">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
JSP - Controller - Service
[EN DESARROLLO]
Se trabajo sobre la pantalla de Registro, en la búsqueda de información
y la suma de costos, faltan método colación y hospedaje.
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/bd/inserts.xlsx
+++ b/src/main/webapp/WEB-INF/bd/inserts.xlsx
@@ -21,6 +21,585 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="201">
   <si>
+    <t>'City Express (Sub-sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ramada Inn (Sub-sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ninguna en particular'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Aguascalientes'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Baja California Sur'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Baja California'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Campeche'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Coahuila de Zaragoza'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Colima'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ap_paterno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ap_materno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Gerardo Martín'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Hernández'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Oliva'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_mesa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_mesa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'contador_visitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perfil_x_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil_x_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>registro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_registro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre_cuerpo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delegacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hospedaje</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_hospedaje</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_salida</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'2016-01-02'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>colacion_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_colacion_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cuerpo_pretende</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado_pretende</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Cocodrilitos'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Abejitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Plantitas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importe_pago</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_participacion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Congresista'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Conferencista'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Coordinador de Mesa'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Secretario de Mesa'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Organizador'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Administrativo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'No aplica'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Lectura'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Presentación en PowerPoint'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parametro_configuracion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Holiday Inn (Sede)'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'31º- 32º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º S.·. N.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º M.·. A.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'33º M.·. Past-A.·.'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grado_pretende</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado_pretende</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'14º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'15º - 18º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'19º - 30º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'31º - 32º'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>' '</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paquete_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_paquete_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_hotel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>precio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_participante</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Lalo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Mario'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Oaxaca'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Puebla'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Querétaro'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>' '</t>
+  </si>
+  <si>
+    <t>' '</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Quintana Roo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'San Luis Potosí'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Sinaloa'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Sonora'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tabasco'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tamaulipas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Tlaxcala'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Veracruz de Ignacio de la Llave'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Yucatán'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Zacatecas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Chiapas'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Chihuahua'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Ciudad de México'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tipo_ponencia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_tipo_ponencia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Durango'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Guanajuato'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Guerrero'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Hidalgo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Jalisco'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'México'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Michoacán de Ocampo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Morelos'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Nayarit'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Nuevo León'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contrasenia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fecha_entrada</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_estado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_grado</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nombre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>descripcion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'gmho'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>activo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_usuario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_perfil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'Gerardo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>'ROLE_ROOT'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,585 +821,6 @@
   </si>
   <si>
     <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'31º- 32º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º S.·. N.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º M.·. A.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'33º M.·. Past-A.·.'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grado_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>precio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'14º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'15º - 18º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'19º - 30º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'31º - 32º'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>' '</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>paquete_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_paquete_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>precio</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Lalo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Mario'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Oaxaca'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Puebla'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Querétaro'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>' '</t>
-  </si>
-  <si>
-    <t>' '</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Quintana Roo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'San Luis Potosí'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Sinaloa'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Sonora'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tabasco'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tamaulipas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Tlaxcala'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Veracruz de Ignacio de la Llave'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Yucatán'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Zacatecas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Chiapas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Chihuahua'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ciudad de México'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_ponencia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_ponencia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Durango'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Guanajuato'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Guerrero'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Hidalgo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Jalisco'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'México'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Michoacán de Ocampo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Morelos'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Nayarit'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Nuevo León'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>contrasenia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_entrada</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'gmho'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Holiday Inn Plaza Universidad (Sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Gerardo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ninguna en particular'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Aguascalientes'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Baja California Sur'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Baja California'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Campeche'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Coahuila de Zaragoza'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Colima'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ap_paterno</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ap_materno</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Gerardo Martín'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Hernández'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Oliva'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_mesa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_mesa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'contador_visitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_estado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>perfil_x_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_perfil_x_usuario</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Ramada Inn Vía Venetto (Sub-sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'City Express Patio Universiad (Sub-sede)'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>registro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_registro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre_cuerpo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delegacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hospedaje</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_hospedaje</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fecha_salida</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'2016-01-02'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>colacion_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_colacion_grado</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_participante</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cuerpo_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_grado_pretende</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Cocodrilitos'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Abejitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Plantitas'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>importe_pago</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id_tipo_participacion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nombre</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>descripcion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>activo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Congresista'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Conferencista'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Coordinador de Mesa'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Secretario de Mesa'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Organizador'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Administrativo'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'No aplica'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Lectura'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>'Presentación en PowerPoint'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hotel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parametro_configuracion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1194,8 +1194,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:J171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G132" sqref="G132"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1205,30 +1205,30 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="B3" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="B4" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1240,19 +1240,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1260,21 +1260,21 @@
     </row>
     <row r="8" spans="1:8">
       <c r="B8" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1286,10 +1286,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1304,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>149</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1319,23 +1319,23 @@
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1358,18 +1358,18 @@
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="B19" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1381,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>137</v>
+        <v>3</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1396,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>139</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1411,7 +1411,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>138</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1426,7 +1426,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>140</v>
+        <v>6</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1441,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1456,7 +1456,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>142</v>
+        <v>8</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1471,7 +1471,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1486,7 +1486,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1501,7 +1501,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1516,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1531,7 +1531,7 @@
         <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1546,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1561,7 +1561,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1576,7 +1576,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1591,7 +1591,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1606,7 +1606,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1621,7 +1621,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1636,7 +1636,7 @@
         <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1651,7 +1651,7 @@
         <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1666,7 +1666,7 @@
         <v>20</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -1681,7 +1681,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1696,7 +1696,7 @@
         <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -1711,7 +1711,7 @@
         <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1726,7 +1726,7 @@
         <v>24</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1741,7 +1741,7 @@
         <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1756,7 +1756,7 @@
         <v>26</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1771,7 +1771,7 @@
         <v>27</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1786,7 +1786,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1801,7 +1801,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1816,7 +1816,7 @@
         <v>30</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1831,7 +1831,7 @@
         <v>31</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1846,7 +1846,7 @@
         <v>32</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1854,21 +1854,21 @@
     </row>
     <row r="54" spans="1:5">
       <c r="B54" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="B55" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E55" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1880,10 +1880,10 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>45</v>
+        <v>190</v>
       </c>
       <c r="D56" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -1898,10 +1898,10 @@
         <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>44</v>
+        <v>189</v>
       </c>
       <c r="D57" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -1916,10 +1916,10 @@
         <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>46</v>
+        <v>191</v>
       </c>
       <c r="D58" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -1934,10 +1934,10 @@
         <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>47</v>
+        <v>192</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -1952,10 +1952,10 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -1970,10 +1970,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D61" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1988,10 +1988,10 @@
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D62" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2006,10 +2006,10 @@
         <v>8</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D63" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2021,21 +2021,21 @@
     </row>
     <row r="66" spans="1:5">
       <c r="B66" t="s">
-        <v>185</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="B67" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="D67" t="s">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="E67" t="s">
-        <v>189</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2047,10 +2047,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>190</v>
+        <v>54</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2065,10 +2065,10 @@
         <v>2</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>191</v>
+        <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2083,10 +2083,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>192</v>
+        <v>56</v>
       </c>
       <c r="D70" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2101,10 +2101,10 @@
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>193</v>
+        <v>57</v>
       </c>
       <c r="D71" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2119,10 +2119,10 @@
         <v>5</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>194</v>
+        <v>58</v>
       </c>
       <c r="D72" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2137,10 +2137,10 @@
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>195</v>
+        <v>59</v>
       </c>
       <c r="D73" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2148,21 +2148,21 @@
     </row>
     <row r="76" spans="1:5">
       <c r="B76" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="B77" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
-        <v>188</v>
+        <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>189</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2174,10 +2174,10 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>196</v>
+        <v>60</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -2192,10 +2192,10 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2210,10 +2210,10 @@
         <v>3</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>198</v>
+        <v>62</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2229,23 +2229,23 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="E84" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2257,10 +2257,10 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>136</v>
+        <v>2</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -2275,10 +2275,10 @@
         <v>2</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>39</v>
+        <v>184</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2293,10 +2293,10 @@
         <v>3</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>40</v>
+        <v>185</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2311,10 +2311,10 @@
         <v>4</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>41</v>
+        <v>186</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2329,10 +2329,10 @@
         <v>5</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -2347,10 +2347,10 @@
         <v>6</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -2366,26 +2366,26 @@
     </row>
     <row r="93" spans="1:6">
       <c r="B93" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:6">
       <c r="B94" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C94" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D94" t="s">
-        <v>151</v>
+        <v>17</v>
       </c>
       <c r="E94" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F94" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2397,10 +2397,10 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E95">
         <v>1500</v>
@@ -2418,10 +2418,10 @@
         <v>2</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E96">
         <v>2000</v>
@@ -2439,10 +2439,10 @@
         <v>3</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E97">
         <v>1700</v>
@@ -2460,10 +2460,10 @@
         <v>4</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E98">
         <v>3400</v>
@@ -2482,30 +2482,30 @@
     </row>
     <row r="101" spans="1:7">
       <c r="B101" t="s">
-        <v>199</v>
+        <v>63</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="B102" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="C102" t="s">
-        <v>187</v>
+        <v>51</v>
       </c>
       <c r="D102" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="str">
         <f>CONCATENATE("INSERT INTO ",B$101," (",B$102,", ",C$102,", ",D$102,") VALUES (",B103,",",C103,",",D103,");" )</f>
-        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (1,'Holiday Inn Plaza Universidad (Sede)',1);</v>
+        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (1,'Holiday Inn (Sede)',1);</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>131</v>
+        <v>65</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -2514,13 +2514,13 @@
     <row r="104" spans="1:7">
       <c r="A104" t="str">
         <f t="shared" ref="A104:A105" si="6">CONCATENATE("INSERT INTO ",B$101," (",B$102,", ",C$102,", ",D$102,") VALUES (",B104,",",C104,",",D104,");" )</f>
-        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (2,'City Express Patio Universiad (Sub-sede)',1);</v>
+        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (2,'City Express (Sub-sede)',1);</v>
       </c>
       <c r="B104">
         <v>2</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>161</v>
+        <v>0</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -2529,13 +2529,13 @@
     <row r="105" spans="1:7">
       <c r="A105" t="str">
         <f t="shared" si="6"/>
-        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (3,'Ramada Inn Vía Venetto (Sub-sede)',1);</v>
+        <v>INSERT INTO hotel (id_hotel, nombre, activo) VALUES (3,'Ramada Inn (Sub-sede)',1);</v>
       </c>
       <c r="B105">
         <v>3</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -2549,28 +2549,28 @@
     </row>
     <row r="108" spans="1:7">
       <c r="B108" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:7">
       <c r="B109" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C109" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E109" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F109" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="G109" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -2585,10 +2585,10 @@
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="F110">
         <v>3520</v>
@@ -2609,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>28</v>
+        <v>173</v>
       </c>
       <c r="F111">
         <v>7040</v>
@@ -2633,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>29</v>
+        <v>174</v>
       </c>
       <c r="F112">
         <v>10560</v>
@@ -2657,10 +2657,10 @@
         <v>2</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>30</v>
+        <v>175</v>
       </c>
       <c r="F113">
         <v>1561</v>
@@ -2681,10 +2681,10 @@
         <v>2</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
       <c r="F114">
         <v>3122</v>
@@ -2705,10 +2705,10 @@
         <v>2</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>29</v>
+        <v>174</v>
       </c>
       <c r="F115">
         <v>4683</v>
@@ -2729,10 +2729,10 @@
         <v>3</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>9</v>
+        <v>154</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="F116">
         <v>895</v>
@@ -2753,10 +2753,10 @@
         <v>3</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>33</v>
+        <v>178</v>
       </c>
       <c r="F117">
         <v>1790</v>
@@ -2777,10 +2777,10 @@
         <v>3</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="F118">
         <v>2685</v>
@@ -2801,10 +2801,10 @@
         <v>3</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>35</v>
+        <v>180</v>
       </c>
       <c r="F119">
         <v>1265</v>
@@ -2825,10 +2825,10 @@
         <v>3</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>36</v>
+        <v>181</v>
       </c>
       <c r="F120">
         <v>2530</v>
@@ -2849,10 +2849,10 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
       <c r="F121">
         <v>3795</v>
@@ -2873,7 +2873,7 @@
     </row>
     <row r="124" spans="1:7">
       <c r="B124" t="s">
-        <v>12</v>
+        <v>157</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2881,19 +2881,19 @@
     </row>
     <row r="125" spans="1:7">
       <c r="B125" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="C125" t="s">
-        <v>14</v>
+        <v>159</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
       <c r="E125" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="F125" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -2905,10 +2905,10 @@
         <v>1</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="E126" s="1">
         <v>1800</v>
@@ -2926,10 +2926,10 @@
         <v>2</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="E127" s="1">
         <v>2300</v>
@@ -2947,10 +2947,10 @@
         <v>3</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="E128" s="1">
         <v>2800</v>
@@ -2971,7 +2971,7 @@
     </row>
     <row r="131" spans="1:6">
       <c r="B131" t="s">
-        <v>48</v>
+        <v>193</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -2979,19 +2979,19 @@
     </row>
     <row r="132" spans="1:6">
       <c r="B132" t="s">
-        <v>49</v>
+        <v>194</v>
       </c>
       <c r="C132" t="s">
-        <v>23</v>
+        <v>168</v>
       </c>
       <c r="D132" t="s">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="E132" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F132" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3003,10 +3003,10 @@
         <v>1</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="E133" s="1">
         <v>1500</v>
@@ -3024,10 +3024,10 @@
         <v>2</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="E134" s="1">
         <v>2000</v>
@@ -3045,10 +3045,10 @@
         <v>3</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>22</v>
+        <v>167</v>
       </c>
       <c r="E135" s="1">
         <v>2500</v>
@@ -3059,21 +3059,21 @@
     </row>
     <row r="138" spans="1:6">
       <c r="B138" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:6">
       <c r="B139" t="s">
-        <v>155</v>
+        <v>21</v>
       </c>
       <c r="C139" t="s">
-        <v>156</v>
+        <v>22</v>
       </c>
       <c r="D139" t="s">
-        <v>157</v>
+        <v>23</v>
       </c>
       <c r="E139" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3085,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D140">
         <v>1</v>
@@ -3096,21 +3096,21 @@
     </row>
     <row r="143" spans="1:6">
       <c r="B143" t="s">
-        <v>1</v>
+        <v>146</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="B144" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="C144" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D144" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E144" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -3125,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -3143,7 +3143,7 @@
         <v>1</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -3151,36 +3151,36 @@
     </row>
     <row r="149" spans="1:10">
       <c r="B149" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
     </row>
     <row r="150" spans="1:10">
       <c r="B150" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="C150" t="s">
-        <v>164</v>
+        <v>28</v>
       </c>
       <c r="D150" t="s">
-        <v>165</v>
+        <v>29</v>
       </c>
       <c r="E150" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="F150" t="s">
-        <v>167</v>
+        <v>31</v>
       </c>
       <c r="G150" t="s">
-        <v>168</v>
+        <v>32</v>
       </c>
       <c r="H150" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="I150" t="s">
-        <v>25</v>
+        <v>170</v>
       </c>
       <c r="J150" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -3198,10 +3198,10 @@
         <v>1</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>180</v>
+        <v>44</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="G151">
         <v>1</v>
@@ -3218,30 +3218,30 @@
     </row>
     <row r="154" spans="1:10">
       <c r="B154" t="s">
-        <v>169</v>
+        <v>33</v>
       </c>
     </row>
     <row r="155" spans="1:10">
       <c r="B155" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="C155" t="s">
+        <v>35</v>
+      </c>
+      <c r="D155" t="s">
+        <v>81</v>
+      </c>
+      <c r="E155" t="s">
+        <v>125</v>
+      </c>
+      <c r="F155" t="s">
+        <v>36</v>
+      </c>
+      <c r="G155" t="s">
         <v>171</v>
       </c>
-      <c r="D155" t="s">
-        <v>71</v>
-      </c>
-      <c r="E155" t="s">
-        <v>115</v>
-      </c>
-      <c r="F155" t="s">
-        <v>172</v>
-      </c>
-      <c r="G155" t="s">
-        <v>26</v>
-      </c>
       <c r="H155" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -3259,10 +3259,10 @@
         <v>1</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>173</v>
+        <v>37</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="G156">
         <v>1</v>
@@ -3273,24 +3273,24 @@
     </row>
     <row r="159" spans="1:10">
       <c r="B159" t="s">
-        <v>174</v>
+        <v>38</v>
       </c>
     </row>
     <row r="160" spans="1:10">
       <c r="B160" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="C160" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="D160" t="s">
-        <v>178</v>
+        <v>42</v>
       </c>
       <c r="E160" t="s">
-        <v>177</v>
+        <v>41</v>
       </c>
       <c r="F160" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -3308,7 +3308,7 @@
         <v>2</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>179</v>
+        <v>43</v>
       </c>
       <c r="F161">
         <v>1</v>
@@ -3316,21 +3316,21 @@
     </row>
     <row r="164" spans="1:6">
       <c r="B164" t="s">
-        <v>182</v>
+        <v>46</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="B165" t="s">
-        <v>183</v>
+        <v>47</v>
       </c>
       <c r="C165" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="D165" t="s">
-        <v>184</v>
+        <v>48</v>
       </c>
       <c r="E165" t="s">
-        <v>55</v>
+        <v>200</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -3353,21 +3353,21 @@
     </row>
     <row r="169" spans="1:6">
       <c r="B169" t="s">
-        <v>200</v>
+        <v>64</v>
       </c>
     </row>
     <row r="170" spans="1:6">
       <c r="B170" t="s">
-        <v>50</v>
+        <v>195</v>
       </c>
       <c r="C170" t="s">
-        <v>51</v>
+        <v>196</v>
       </c>
       <c r="D170" t="s">
-        <v>52</v>
+        <v>197</v>
       </c>
       <c r="E170" t="s">
-        <v>53</v>
+        <v>198</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -3379,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="D171">
         <v>0</v>

</xml_diff>